<commit_message>
relaciones puestos trabajo modificado
</commit_message>
<xml_diff>
--- a/LOD-datasets/Datasets Linked Data.xlsx
+++ b/LOD-datasets/Datasets Linked Data.xlsx
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Relación de puestos de trabajo</t>
-  </si>
-  <si>
-    <t>http://opendata.euskadi.eus/catalogo/-/relaciones-de-puestos-de-trabajo-de-los-departamentos-y-organismos-autonomos-de-la-administracion-de-la-comunidad-autonoma/</t>
   </si>
   <si>
     <t>Mediciones del polen</t>
@@ -87,12 +84,15 @@
   <si>
     <t>http://opendata.euskadi.eus/catalogo/-/registro-de-contratos-del-sector-publico-de-euskadi/</t>
   </si>
+  <si>
+    <t xml:space="preserve">http://opendata.euskadi.eus/catalogo/-/relacion-de-puestos-de-trabajo-rpt-de-los-departamentos-y-organismos-autonomos-de-la-administracion-de-la-comunidad-autonoma/ </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -121,6 +121,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -158,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -170,6 +176,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -478,7 +485,7 @@
   <dimension ref="A1:X987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -552,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -582,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -612,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -639,10 +646,10 @@
     </row>
     <row r="6" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -669,10 +676,10 @@
     </row>
     <row r="7" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -699,10 +706,10 @@
     </row>
     <row r="8" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -729,10 +736,10 @@
     </row>
     <row r="9" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -759,10 +766,10 @@
     </row>
     <row r="10" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -789,10 +796,10 @@
     </row>
     <row r="11" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -819,10 +826,10 @@
     </row>
     <row r="12" spans="1:24" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -26217,9 +26224,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26337,25 +26347,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4039134-C340-4F59-B4AB-A013EC5784B1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABC685D-9297-4C18-9F3B-8598B1D56238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -26377,9 +26377,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABC685D-9297-4C18-9F3B-8598B1D56238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4039134-C340-4F59-B4AB-A013EC5784B1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>